<commit_message>
renamed column of data
</commit_message>
<xml_diff>
--- a/Data/body_temp.xlsx
+++ b/Data/body_temp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B64558-D78B-4644-B2AD-D7B46849B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E069BDDB-EE84-4D65-A2CE-C25981574355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,10 +77,10 @@
     <t>gender</t>
   </si>
   <si>
-    <t>body_temp</t>
+    <t>source</t>
   </si>
   <si>
-    <t>source</t>
+    <t>temperature</t>
   </si>
 </sst>
 </file>
@@ -459,20 +459,23 @@
   <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>